<commit_message>
Se agrega carpetas e informe final
</commit_message>
<xml_diff>
--- a/challenge_1/tienda2/tienda_2.xlsx
+++ b/challenge_1/tienda2/tienda_2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\challenge_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\challenge_1\challenge_1\tienda2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4B02B2-9B54-4D73-94D2-E705A5D56F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D540EEA-FC8C-4CEC-A7EC-1649048A92FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,17 @@
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3425,6 +3436,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3452,8 +3466,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3758,9 +3773,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2360"/>
+  <dimension ref="A1:L2361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2337" workbookViewId="0">
+      <selection activeCell="D2361" sqref="D2361"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -93453,8 +93470,15 @@
         <v>-75.563590000000005</v>
       </c>
     </row>
+    <row r="2361" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D2361" s="1">
+        <f>SUM(D2:D2360)</f>
+        <v>59485100</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>